<commit_message>
IKB check and converted to OSG
</commit_message>
<xml_diff>
--- a/clo.xlsx
+++ b/clo.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="945" yWindow="1155" windowWidth="27555" windowHeight="13065"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2193" uniqueCount="299">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2191" uniqueCount="299">
   <si>
     <t>Monday  </t>
   </si>
@@ -918,7 +923,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -968,6 +973,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1015,7 +1023,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1048,9 +1056,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1083,6 +1108,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1261,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D796"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A307" workbookViewId="0">
-      <selection activeCell="G346" sqref="G346"/>
+    <sheetView tabSelected="1" topLeftCell="A283" workbookViewId="0">
+      <selection activeCell="C295" sqref="C295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5349,38 +5391,22 @@
         <v>126</v>
       </c>
       <c r="B293" s="2">
-        <v>0.41666666666666669</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C293" s="2">
-        <v>0.47916666666666669</v>
-      </c>
-      <c r="D293" t="s">
-        <v>3</v>
+        <v>0.6875</v>
       </c>
     </row>
     <row r="294" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B294" s="2">
-        <v>0.60416666666666663</v>
-      </c>
-      <c r="C294" s="2">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="D294" t="s">
-        <v>3</v>
-      </c>
+      <c r="B294" s="2"/>
+      <c r="C294" s="2"/>
     </row>
     <row r="295" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B295" s="2">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="C295" s="2">
-        <v>0.6875</v>
       </c>
       <c r="D295" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Name changes for variables
</commit_message>
<xml_diff>
--- a/clo.xlsx
+++ b/clo.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="10290"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="264">
   <si>
     <t>Friday  </t>
   </si>
@@ -813,7 +818,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -855,6 +860,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -903,7 +911,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -936,9 +944,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -971,6 +996,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1150,7 +1192,7 @@
   <dimension ref="A1:E363"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="C154" sqref="C154"/>
+      <selection activeCell="D154" sqref="A154:D155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3733,18 +3775,8 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>14</v>
-      </c>
-      <c r="B154" s="1">
-        <v>0.5625</v>
-      </c>
-      <c r="C154" s="1">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="D154" t="s">
-        <v>126</v>
-      </c>
+      <c r="B154" s="1"/>
+      <c r="C154" s="1"/>
       <c r="E154" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Added Headers. Need to test the clo with other outlers still
</commit_message>
<xml_diff>
--- a/clo.xlsx
+++ b/clo.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jhan\Documents\Visual Studio 2015\Projects\ClassOpsLogCreator\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="10290"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1416" uniqueCount="264">
   <si>
     <t>Friday  </t>
   </si>
@@ -818,7 +813,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -860,9 +855,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -911,7 +903,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -944,26 +936,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -996,23 +971,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1189,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E363"/>
+  <dimension ref="A1:E361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
-      <selection activeCell="D154" sqref="A154:D155"/>
+    <sheetView tabSelected="1" topLeftCell="A217" workbookViewId="0">
+      <selection activeCell="G270" sqref="G270"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1269,8 +1227,18 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
       <c r="E6" t="s">
         <v>4</v>
       </c>
@@ -3775,34 +3743,68 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
+      <c r="A154" t="s">
+        <v>14</v>
+      </c>
+      <c r="B154" t="s">
+        <v>2</v>
+      </c>
+      <c r="C154" t="s">
+        <v>2</v>
+      </c>
+      <c r="D154" t="s">
+        <v>3</v>
+      </c>
       <c r="E154" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>127</v>
+      </c>
+      <c r="B155" s="1">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C155" s="1">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D155" t="s">
+        <v>128</v>
+      </c>
       <c r="E155" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>14</v>
+      </c>
+      <c r="B156" t="s">
+        <v>2</v>
+      </c>
+      <c r="C156" t="s">
+        <v>2</v>
+      </c>
+      <c r="D156" t="s">
+        <v>3</v>
+      </c>
       <c r="E156" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B157" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.375</v>
       </c>
       <c r="C157" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D157" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="E157" t="s">
         <v>11</v>
@@ -3827,16 +3829,16 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B159" s="1">
-        <v>0.375</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="C159" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D159" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E159" t="s">
         <v>11</v>
@@ -3861,7 +3863,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B161" s="1">
         <v>0.35416666666666669</v>
@@ -3895,16 +3897,16 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B163" s="1">
-        <v>0.35416666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="C163" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D163" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E163" t="s">
         <v>11</v>
@@ -3929,7 +3931,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B165" s="1">
         <v>0.375</v>
@@ -3963,7 +3965,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B167" s="1">
         <v>0.375</v>
@@ -3972,7 +3974,7 @@
         <v>0.66666666666666663</v>
       </c>
       <c r="D167" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E167" t="s">
         <v>11</v>
@@ -3997,16 +3999,16 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B169" s="1">
-        <v>0.375</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="C169" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D169" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E169" t="s">
         <v>11</v>
@@ -4031,16 +4033,16 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B171" s="1">
-        <v>0.35416666666666669</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="C171" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="D171" t="s">
-        <v>132</v>
+        <v>69</v>
       </c>
       <c r="E171" t="s">
         <v>11</v>
@@ -4065,13 +4067,13 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B173" s="1">
         <v>0.29166666666666669</v>
       </c>
       <c r="C173" s="1">
-        <v>0.99930555555555556</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D173" t="s">
         <v>69</v>
@@ -4152,14 +4154,14 @@
       <c r="A178" t="s">
         <v>14</v>
       </c>
-      <c r="B178" t="s">
-        <v>2</v>
-      </c>
-      <c r="C178" t="s">
-        <v>2</v>
+      <c r="B178" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C178" s="1">
+        <v>0.625</v>
       </c>
       <c r="D178" t="s">
-        <v>3</v>
+        <v>142</v>
       </c>
       <c r="E178" t="s">
         <v>4</v>
@@ -4167,16 +4169,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>141</v>
-      </c>
-      <c r="B179" s="1">
-        <v>0.29166666666666669</v>
-      </c>
-      <c r="C179" s="1">
-        <v>0.35416666666666669</v>
+        <v>14</v>
+      </c>
+      <c r="B179" t="s">
+        <v>2</v>
+      </c>
+      <c r="C179" t="s">
+        <v>2</v>
       </c>
       <c r="D179" t="s">
-        <v>69</v>
+        <v>3</v>
       </c>
       <c r="E179" t="s">
         <v>4</v>
@@ -4184,16 +4186,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>14</v>
+        <v>143</v>
       </c>
       <c r="B180" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="C180" s="1">
-        <v>0.625</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="D180" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="E180" t="s">
         <v>11</v>
@@ -4218,16 +4220,16 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B182" s="1">
-        <v>0.29166666666666669</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="C182" s="1">
-        <v>0.99930555555555556</v>
+        <v>0.4375</v>
       </c>
       <c r="D182" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="E182" t="s">
         <v>4</v>
@@ -4237,14 +4239,14 @@
       <c r="A183" t="s">
         <v>14</v>
       </c>
-      <c r="B183" t="s">
-        <v>2</v>
-      </c>
-      <c r="C183" t="s">
-        <v>2</v>
+      <c r="B183" s="1">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C183" s="1">
+        <v>0.85416666666666663</v>
       </c>
       <c r="D183" t="s">
-        <v>3</v>
+        <v>146</v>
       </c>
       <c r="E183" t="s">
         <v>11</v>
@@ -4252,16 +4254,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>144</v>
-      </c>
-      <c r="B184" s="1">
-        <v>0.35416666666666669</v>
-      </c>
-      <c r="C184" s="1">
-        <v>0.4375</v>
+        <v>14</v>
+      </c>
+      <c r="B184" t="s">
+        <v>2</v>
+      </c>
+      <c r="C184" t="s">
+        <v>2</v>
       </c>
       <c r="D184" t="s">
-        <v>145</v>
+        <v>3</v>
       </c>
       <c r="E184" t="s">
         <v>4</v>
@@ -4269,16 +4271,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>14</v>
+        <v>147</v>
       </c>
       <c r="B185" s="1">
-        <v>0.77083333333333337</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="C185" s="1">
-        <v>0.85416666666666663</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D185" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="E185" t="s">
         <v>11</v>
@@ -4288,14 +4290,14 @@
       <c r="A186" t="s">
         <v>14</v>
       </c>
-      <c r="B186" t="s">
-        <v>2</v>
-      </c>
-      <c r="C186" t="s">
-        <v>2</v>
+      <c r="B186" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C186" s="1">
+        <v>0.60416666666666663</v>
       </c>
       <c r="D186" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="E186" t="s">
         <v>11</v>
@@ -4303,16 +4305,16 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>147</v>
+        <v>14</v>
       </c>
       <c r="B187" s="1">
-        <v>0.29166666666666669</v>
+        <v>0.625</v>
       </c>
       <c r="C187" s="1">
-        <v>0.35416666666666669</v>
+        <v>0.6875</v>
       </c>
       <c r="D187" t="s">
-        <v>69</v>
+        <v>149</v>
       </c>
       <c r="E187" t="s">
         <v>11</v>
@@ -4322,14 +4324,14 @@
       <c r="A188" t="s">
         <v>14</v>
       </c>
-      <c r="B188" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="C188" s="1">
-        <v>0.60416666666666663</v>
+      <c r="B188" t="s">
+        <v>2</v>
+      </c>
+      <c r="C188" t="s">
+        <v>2</v>
       </c>
       <c r="D188" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="E188" t="s">
         <v>4</v>
@@ -4337,16 +4339,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>14</v>
+        <v>150</v>
       </c>
       <c r="B189" s="1">
-        <v>0.625</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="C189" s="1">
-        <v>0.6875</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="D189" t="s">
-        <v>149</v>
+        <v>69</v>
       </c>
       <c r="E189" t="s">
         <v>11</v>
@@ -4371,16 +4373,16 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B191" s="1">
-        <v>0.29166666666666669</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C191" s="1">
-        <v>0.35416666666666669</v>
+        <v>0.72222222222222221</v>
       </c>
       <c r="D191" t="s">
-        <v>69</v>
+        <v>152</v>
       </c>
       <c r="E191" t="s">
         <v>11</v>
@@ -4405,16 +4407,16 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B193" s="1">
-        <v>0.58333333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="C193" s="1">
-        <v>0.72222222222222221</v>
+        <v>0.67361111111111116</v>
       </c>
       <c r="D193" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="E193" t="s">
         <v>4</v>
@@ -4439,16 +4441,16 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B195" s="1">
-        <v>0.5625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C195" s="1">
-        <v>0.67361111111111116</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D195" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E195" t="s">
         <v>11</v>
@@ -4458,14 +4460,14 @@
       <c r="A196" t="s">
         <v>14</v>
       </c>
-      <c r="B196" t="s">
-        <v>2</v>
-      </c>
-      <c r="C196" t="s">
-        <v>2</v>
+      <c r="B196" s="1">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C196" s="1">
+        <v>0.91319444444444453</v>
       </c>
       <c r="D196" t="s">
-        <v>3</v>
+        <v>157</v>
       </c>
       <c r="E196" t="s">
         <v>11</v>
@@ -4473,16 +4475,16 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>155</v>
-      </c>
-      <c r="B197" s="1">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C197" s="1">
-        <v>0.70833333333333337</v>
+        <v>14</v>
+      </c>
+      <c r="B197" t="s">
+        <v>2</v>
+      </c>
+      <c r="C197" t="s">
+        <v>2</v>
       </c>
       <c r="D197" t="s">
-        <v>156</v>
+        <v>3</v>
       </c>
       <c r="E197" t="s">
         <v>4</v>
@@ -4490,16 +4492,16 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>14</v>
+        <v>158</v>
       </c>
       <c r="B198" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="C198" s="1">
         <v>0.72916666666666663</v>
       </c>
-      <c r="C198" s="1">
-        <v>0.91319444444444453</v>
-      </c>
       <c r="D198" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E198" t="s">
         <v>11</v>
@@ -4524,16 +4526,16 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B200" s="1">
-        <v>0.5625</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C200" s="1">
-        <v>0.72916666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="D200" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E200" t="s">
         <v>4</v>
@@ -4558,16 +4560,16 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B202" s="1">
         <v>0.58333333333333337</v>
       </c>
       <c r="C202" s="1">
-        <v>0.75</v>
+        <v>0.6875</v>
       </c>
       <c r="D202" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E202" t="s">
         <v>11</v>
@@ -4577,14 +4579,14 @@
       <c r="A203" t="s">
         <v>14</v>
       </c>
-      <c r="B203" t="s">
-        <v>2</v>
-      </c>
-      <c r="C203" t="s">
-        <v>2</v>
+      <c r="B203" s="1">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C203" s="1">
+        <v>0.84027777777777779</v>
       </c>
       <c r="D203" t="s">
-        <v>3</v>
+        <v>159</v>
       </c>
       <c r="E203" t="s">
         <v>11</v>
@@ -4592,16 +4594,16 @@
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>162</v>
-      </c>
-      <c r="B204" s="1">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="C204" s="1">
-        <v>0.6875</v>
+        <v>14</v>
+      </c>
+      <c r="B204" t="s">
+        <v>2</v>
+      </c>
+      <c r="C204" t="s">
+        <v>2</v>
       </c>
       <c r="D204" t="s">
-        <v>163</v>
+        <v>3</v>
       </c>
       <c r="E204" t="s">
         <v>4</v>
@@ -4609,16 +4611,16 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>14</v>
+        <v>164</v>
       </c>
       <c r="B205" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C205" s="1">
         <v>0.70833333333333337</v>
       </c>
-      <c r="C205" s="1">
-        <v>0.84027777777777779</v>
-      </c>
       <c r="D205" t="s">
-        <v>159</v>
+        <v>165</v>
       </c>
       <c r="E205" t="s">
         <v>11</v>
@@ -4643,16 +4645,16 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B207" s="1">
         <v>0.54166666666666663</v>
       </c>
       <c r="C207" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="D207" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E207" t="s">
         <v>4</v>
@@ -4677,16 +4679,16 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B209" s="1">
-        <v>0.54166666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="C209" s="1">
-        <v>0.72916666666666663</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D209" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="E209" t="s">
         <v>11</v>
@@ -4711,7 +4713,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B211" s="1">
         <v>0.375</v>
@@ -4745,16 +4747,16 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B213" s="1">
-        <v>0.375</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="C213" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.4375</v>
       </c>
       <c r="D213" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E213" t="s">
         <v>11</v>
@@ -4779,16 +4781,16 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B215" s="1">
-        <v>0.35416666666666669</v>
+        <v>0.375</v>
       </c>
       <c r="C215" s="1">
-        <v>0.4375</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D215" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E215" t="s">
         <v>11</v>
@@ -4813,16 +4815,16 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B217" s="1">
-        <v>0.375</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C217" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D217" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="E217" t="s">
         <v>11</v>
@@ -4847,16 +4849,16 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B219" s="1">
-        <v>0.47916666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C219" s="1">
-        <v>0.60416666666666663</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="D219" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="E219" t="s">
         <v>11</v>
@@ -4881,16 +4883,16 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B221" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C221" s="1">
-        <v>0.99930555555555556</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D221" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="E221" t="s">
         <v>11</v>
@@ -4915,16 +4917,16 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B223" s="1">
         <v>0.47916666666666669</v>
       </c>
       <c r="C223" s="1">
-        <v>0.60416666666666663</v>
+        <v>0.5625</v>
       </c>
       <c r="D223" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="E223" t="s">
         <v>11</v>
@@ -4949,7 +4951,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B225" s="1">
         <v>0.47916666666666669</v>
@@ -4983,13 +4985,13 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B227" s="1">
-        <v>0.47916666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C227" s="1">
-        <v>0.5625</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="D227" t="s">
         <v>169</v>
@@ -5017,16 +5019,16 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B229" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C229" s="1">
-        <v>0.99930555555555556</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D229" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="E229" t="s">
         <v>4</v>
@@ -5051,16 +5053,16 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B231" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.625</v>
       </c>
       <c r="C231" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.75</v>
       </c>
       <c r="D231" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="E231" t="s">
         <v>11</v>
@@ -5085,16 +5087,16 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B233" s="1">
-        <v>0.625</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="C233" s="1">
-        <v>0.75</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D233" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="E233" t="s">
         <v>11</v>
@@ -5119,16 +5121,16 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B235" s="1">
         <v>0.35416666666666669</v>
       </c>
       <c r="C235" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="D235" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E235" t="s">
         <v>11</v>
@@ -5153,16 +5155,16 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B237" s="1">
-        <v>0.35416666666666669</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C237" s="1">
-        <v>0.47916666666666669</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D237" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E237" t="s">
         <v>11</v>
@@ -5187,16 +5189,16 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B239" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="C239" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D239" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E239" t="s">
         <v>11</v>
@@ -5221,16 +5223,16 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B241" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="C241" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.625</v>
       </c>
       <c r="D241" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E241" t="s">
         <v>11</v>
@@ -5255,16 +5257,16 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B243" s="1">
-        <v>0.375</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="C243" s="1">
-        <v>0.625</v>
+        <v>0.6875</v>
       </c>
       <c r="D243" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="E243" t="s">
         <v>11</v>
@@ -5289,7 +5291,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B245" s="1">
         <v>0.35416666666666669</v>
@@ -5298,7 +5300,7 @@
         <v>0.6875</v>
       </c>
       <c r="D245" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="E245" t="s">
         <v>11</v>
@@ -5323,16 +5325,16 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="B247" s="1">
-        <v>0.35416666666666669</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="C247" s="1">
-        <v>0.6875</v>
+        <v>0.5</v>
       </c>
       <c r="D247" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E247" t="s">
         <v>4</v>
@@ -5357,16 +5359,16 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B249" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="C249" s="1">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D249" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="E249" t="s">
         <v>4</v>
@@ -5391,16 +5393,16 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B251" s="1">
-        <v>0.6875</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C251" s="1">
         <v>0</v>
       </c>
       <c r="D251" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E251" t="s">
         <v>4</v>
@@ -5425,16 +5427,16 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B253" s="1">
-        <v>0.64583333333333337</v>
+        <v>0.375</v>
       </c>
       <c r="C253" s="1">
-        <v>0</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D253" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E253" t="s">
         <v>4</v>
@@ -5459,16 +5461,16 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="B255" s="1">
-        <v>0.375</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="C255" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="D255" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="E255" t="s">
         <v>4</v>
@@ -5493,16 +5495,16 @@
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B257" s="1">
-        <v>0.58333333333333337</v>
+        <v>0.3125</v>
       </c>
       <c r="C257" s="1">
-        <v>0.64583333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D257" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="E257" t="s">
         <v>11</v>
@@ -5512,14 +5514,14 @@
       <c r="A258" t="s">
         <v>14</v>
       </c>
-      <c r="B258" t="s">
-        <v>2</v>
-      </c>
-      <c r="C258" t="s">
-        <v>2</v>
+      <c r="B258" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C258" s="1">
+        <v>0.66666666666666663</v>
       </c>
       <c r="D258" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="E258" t="s">
         <v>11</v>
@@ -5527,16 +5529,16 @@
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>210</v>
+        <v>14</v>
       </c>
       <c r="B259" s="1">
-        <v>0.3125</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C259" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D259" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E259" t="s">
         <v>4</v>
@@ -5546,14 +5548,14 @@
       <c r="A260" t="s">
         <v>14</v>
       </c>
-      <c r="B260" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C260" s="1">
-        <v>0.66666666666666663</v>
+      <c r="B260" t="s">
+        <v>2</v>
+      </c>
+      <c r="C260" t="s">
+        <v>2</v>
       </c>
       <c r="D260" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="E260" t="s">
         <v>4</v>
@@ -5561,16 +5563,16 @@
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="B261" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.3125</v>
       </c>
       <c r="C261" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D261" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E261" t="s">
         <v>11</v>
@@ -5580,14 +5582,14 @@
       <c r="A262" t="s">
         <v>14</v>
       </c>
-      <c r="B262" t="s">
-        <v>2</v>
-      </c>
-      <c r="C262" t="s">
-        <v>2</v>
+      <c r="B262" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C262" s="1">
+        <v>0.66666666666666663</v>
       </c>
       <c r="D262" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="E262" t="s">
         <v>11</v>
@@ -5595,16 +5597,16 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>210</v>
+        <v>14</v>
       </c>
       <c r="B263" s="1">
-        <v>0.3125</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C263" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D263" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E263" t="s">
         <v>4</v>
@@ -5614,14 +5616,14 @@
       <c r="A264" t="s">
         <v>14</v>
       </c>
-      <c r="B264" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C264" s="1">
-        <v>0.66666666666666663</v>
+      <c r="B264" t="s">
+        <v>2</v>
+      </c>
+      <c r="C264" t="s">
+        <v>2</v>
       </c>
       <c r="D264" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="E264" t="s">
         <v>4</v>
@@ -5629,16 +5631,16 @@
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>14</v>
+        <v>210</v>
       </c>
       <c r="B265" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.3125</v>
       </c>
       <c r="C265" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D265" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E265" t="s">
         <v>11</v>
@@ -5648,14 +5650,14 @@
       <c r="A266" t="s">
         <v>14</v>
       </c>
-      <c r="B266" t="s">
-        <v>2</v>
-      </c>
-      <c r="C266" t="s">
-        <v>2</v>
+      <c r="B266" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C266" s="1">
+        <v>0.66666666666666663</v>
       </c>
       <c r="D266" t="s">
-        <v>3</v>
+        <v>148</v>
       </c>
       <c r="E266" t="s">
         <v>11</v>
@@ -5663,16 +5665,16 @@
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>210</v>
+        <v>14</v>
       </c>
       <c r="B267" s="1">
-        <v>0.3125</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="C267" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D267" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E267" t="s">
         <v>4</v>
@@ -5682,14 +5684,14 @@
       <c r="A268" t="s">
         <v>14</v>
       </c>
-      <c r="B268" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C268" s="1">
-        <v>0.66666666666666663</v>
+      <c r="B268" t="s">
+        <v>2</v>
+      </c>
+      <c r="C268" t="s">
+        <v>2</v>
       </c>
       <c r="D268" t="s">
-        <v>148</v>
+        <v>3</v>
       </c>
       <c r="E268" t="s">
         <v>4</v>
@@ -5697,16 +5699,16 @@
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>14</v>
+        <v>213</v>
       </c>
       <c r="B269" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.3125</v>
       </c>
       <c r="C269" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D269" t="s">
-        <v>212</v>
+        <v>145</v>
       </c>
       <c r="E269" t="s">
         <v>4</v>
@@ -5716,14 +5718,14 @@
       <c r="A270" t="s">
         <v>14</v>
       </c>
-      <c r="B270" t="s">
-        <v>2</v>
-      </c>
-      <c r="C270" t="s">
-        <v>2</v>
+      <c r="B270" s="1">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="C270" s="1">
+        <v>0.5625</v>
       </c>
       <c r="D270" t="s">
-        <v>3</v>
+        <v>214</v>
       </c>
       <c r="E270" t="s">
         <v>4</v>
@@ -5731,16 +5733,16 @@
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>213</v>
+        <v>14</v>
       </c>
       <c r="B271" s="1">
-        <v>0.3125</v>
+        <v>0.5625</v>
       </c>
       <c r="C271" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="D271" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E271" t="s">
         <v>11</v>
@@ -5751,13 +5753,13 @@
         <v>14</v>
       </c>
       <c r="B272" s="1">
-        <v>0.47916666666666669</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="C272" s="1">
-        <v>0.5625</v>
+        <v>0.6875</v>
       </c>
       <c r="D272" t="s">
-        <v>214</v>
+        <v>149</v>
       </c>
       <c r="E272" t="s">
         <v>11</v>
@@ -5768,13 +5770,13 @@
         <v>14</v>
       </c>
       <c r="B273" s="1">
-        <v>0.5625</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="C273" s="1">
-        <v>0.64583333333333337</v>
+        <v>0.79166666666666663</v>
       </c>
       <c r="D273" t="s">
-        <v>148</v>
+        <v>214</v>
       </c>
       <c r="E273" t="s">
         <v>4</v>
@@ -5784,14 +5786,14 @@
       <c r="A274" t="s">
         <v>14</v>
       </c>
-      <c r="B274" s="1">
-        <v>0.64583333333333337</v>
-      </c>
-      <c r="C274" s="1">
-        <v>0.6875</v>
+      <c r="B274" t="s">
+        <v>2</v>
+      </c>
+      <c r="C274" t="s">
+        <v>2</v>
       </c>
       <c r="D274" t="s">
-        <v>149</v>
+        <v>3</v>
       </c>
       <c r="E274" t="s">
         <v>4</v>
@@ -5799,16 +5801,16 @@
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>14</v>
+        <v>215</v>
       </c>
       <c r="B275" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.375</v>
       </c>
       <c r="C275" s="1">
-        <v>0.79166666666666663</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D275" t="s">
-        <v>214</v>
+        <v>148</v>
       </c>
       <c r="E275" t="s">
         <v>11</v>
@@ -5867,16 +5869,16 @@
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B279" s="1">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="C279" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="D279" t="s">
-        <v>148</v>
+        <v>217</v>
       </c>
       <c r="E279" t="s">
         <v>4</v>
@@ -5901,16 +5903,16 @@
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B281" s="1">
-        <v>0.25</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C281" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.54166666666666663</v>
       </c>
       <c r="D281" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E281" t="s">
         <v>11</v>
@@ -5920,14 +5922,14 @@
       <c r="A282" t="s">
         <v>14</v>
       </c>
-      <c r="B282" t="s">
-        <v>2</v>
-      </c>
-      <c r="C282" t="s">
-        <v>2</v>
+      <c r="B282" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="C282" s="1">
+        <v>0.83333333333333337</v>
       </c>
       <c r="D282" t="s">
-        <v>3</v>
+        <v>220</v>
       </c>
       <c r="E282" t="s">
         <v>4</v>
@@ -5935,16 +5937,16 @@
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>218</v>
-      </c>
-      <c r="B283" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C283" s="1">
-        <v>0.54166666666666663</v>
+        <v>14</v>
+      </c>
+      <c r="B283" t="s">
+        <v>2</v>
+      </c>
+      <c r="C283" t="s">
+        <v>2</v>
       </c>
       <c r="D283" t="s">
-        <v>219</v>
+        <v>3</v>
       </c>
       <c r="E283" t="s">
         <v>4</v>
@@ -5952,16 +5954,16 @@
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="B284" s="1">
-        <v>0.54166666666666663</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C284" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D284" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="E284" t="s">
         <v>4</v>
@@ -5971,14 +5973,14 @@
       <c r="A285" t="s">
         <v>14</v>
       </c>
-      <c r="B285" t="s">
-        <v>2</v>
-      </c>
-      <c r="C285" t="s">
-        <v>2</v>
+      <c r="B285" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C285" s="1">
+        <v>0.83333333333333337</v>
       </c>
       <c r="D285" t="s">
-        <v>3</v>
+        <v>223</v>
       </c>
       <c r="E285" t="s">
         <v>4</v>
@@ -5986,16 +5988,16 @@
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>221</v>
-      </c>
-      <c r="B286" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C286" s="1">
-        <v>0.41666666666666669</v>
+        <v>14</v>
+      </c>
+      <c r="B286" t="s">
+        <v>2</v>
+      </c>
+      <c r="C286" t="s">
+        <v>2</v>
       </c>
       <c r="D286" t="s">
-        <v>222</v>
+        <v>3</v>
       </c>
       <c r="E286" t="s">
         <v>4</v>
@@ -6003,16 +6005,16 @@
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>14</v>
+        <v>221</v>
       </c>
       <c r="B287" s="1">
-        <v>0.75</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C287" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D287" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E287" t="s">
         <v>4</v>
@@ -6022,14 +6024,14 @@
       <c r="A288" t="s">
         <v>14</v>
       </c>
-      <c r="B288" t="s">
-        <v>2</v>
-      </c>
-      <c r="C288" t="s">
-        <v>2</v>
+      <c r="B288" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="C288" s="1">
+        <v>0.83333333333333337</v>
       </c>
       <c r="D288" t="s">
-        <v>3</v>
+        <v>223</v>
       </c>
       <c r="E288" t="s">
         <v>4</v>
@@ -6037,16 +6039,16 @@
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>221</v>
-      </c>
-      <c r="B289" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C289" s="1">
-        <v>0.41666666666666669</v>
+        <v>14</v>
+      </c>
+      <c r="B289" t="s">
+        <v>2</v>
+      </c>
+      <c r="C289" t="s">
+        <v>2</v>
       </c>
       <c r="D289" t="s">
-        <v>222</v>
+        <v>3</v>
       </c>
       <c r="E289" t="s">
         <v>4</v>
@@ -6054,16 +6056,16 @@
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>14</v>
+        <v>224</v>
       </c>
       <c r="B290" s="1">
-        <v>0.75</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="C290" s="1">
-        <v>0.83333333333333337</v>
+        <v>0.5625</v>
       </c>
       <c r="D290" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E290" t="s">
         <v>11</v>
@@ -6258,16 +6260,16 @@
     </row>
     <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B302" s="1">
-        <v>0.47916666666666669</v>
+        <v>0.35416666666666669</v>
       </c>
       <c r="C302" s="1">
-        <v>0.5625</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="D302" t="s">
-        <v>225</v>
+        <v>132</v>
       </c>
       <c r="E302" t="s">
         <v>11</v>
@@ -6292,16 +6294,16 @@
     </row>
     <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B304" s="1">
-        <v>0.35416666666666669</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="C304" s="1">
-        <v>0.70833333333333337</v>
+        <v>0.52083333333333337</v>
       </c>
       <c r="D304" t="s">
-        <v>132</v>
+        <v>228</v>
       </c>
       <c r="E304" t="s">
         <v>11</v>
@@ -6326,16 +6328,16 @@
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B306" s="1">
-        <v>0.39583333333333331</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C306" s="1">
-        <v>0.52083333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D306" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="E306" t="s">
         <v>11</v>
@@ -6360,16 +6362,16 @@
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B308" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C308" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.5</v>
       </c>
       <c r="D308" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E308" t="s">
         <v>4</v>
@@ -6379,14 +6381,14 @@
       <c r="A309" t="s">
         <v>14</v>
       </c>
-      <c r="B309" t="s">
-        <v>2</v>
-      </c>
-      <c r="C309" t="s">
-        <v>2</v>
+      <c r="B309" s="1">
+        <v>0.5625</v>
+      </c>
+      <c r="C309" s="1">
+        <v>0.64583333333333337</v>
       </c>
       <c r="D309" t="s">
-        <v>3</v>
+        <v>233</v>
       </c>
       <c r="E309" t="s">
         <v>11</v>
@@ -6394,16 +6396,16 @@
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>231</v>
-      </c>
-      <c r="B310" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="C310" s="1">
-        <v>0.5</v>
+        <v>14</v>
+      </c>
+      <c r="B310" t="s">
+        <v>2</v>
+      </c>
+      <c r="C310" t="s">
+        <v>2</v>
       </c>
       <c r="D310" t="s">
-        <v>232</v>
+        <v>3</v>
       </c>
       <c r="E310" t="s">
         <v>4</v>
@@ -6411,16 +6413,16 @@
     </row>
     <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>14</v>
+        <v>234</v>
       </c>
       <c r="B311" s="1">
-        <v>0.5625</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C311" s="1">
-        <v>0.64583333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D311" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E311" t="s">
         <v>11</v>
@@ -6445,7 +6447,7 @@
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B313" s="1">
         <v>0.33333333333333331</v>
@@ -6479,7 +6481,7 @@
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="B315" s="1">
         <v>0.33333333333333331</v>
@@ -6513,16 +6515,16 @@
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B317" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.5625</v>
       </c>
       <c r="C317" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.64583333333333337</v>
       </c>
       <c r="D317" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E317" t="s">
         <v>4</v>
@@ -6547,16 +6549,16 @@
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B319" s="1">
-        <v>0.5625</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C319" s="1">
-        <v>0.64583333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D319" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E319" t="s">
         <v>11</v>
@@ -6581,7 +6583,7 @@
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B321" s="1">
         <v>0.33333333333333331</v>
@@ -6615,7 +6617,7 @@
     </row>
     <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B323" s="1">
         <v>0.33333333333333331</v>
@@ -6649,7 +6651,7 @@
     </row>
     <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B325" s="1">
         <v>0.33333333333333331</v>
@@ -6683,16 +6685,16 @@
     </row>
     <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B327" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="C327" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="D327" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="E327" t="s">
         <v>11</v>
@@ -6717,16 +6719,16 @@
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="B329" s="1">
-        <v>0.41666666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C329" s="1">
-        <v>0.58333333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D329" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="E329" t="s">
         <v>11</v>
@@ -6751,16 +6753,16 @@
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B331" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="C331" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.91666666666666663</v>
       </c>
       <c r="D331" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="E331" t="s">
         <v>11</v>
@@ -6785,16 +6787,16 @@
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B333" s="1">
-        <v>0.29166666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C333" s="1">
-        <v>0.91666666666666663</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D333" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="E333" t="s">
         <v>11</v>
@@ -6819,7 +6821,7 @@
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B335" s="1">
         <v>0.33333333333333331</v>
@@ -6853,7 +6855,7 @@
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B337" s="1">
         <v>0.33333333333333331</v>
@@ -6887,16 +6889,16 @@
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B339" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="C339" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.99930555555555556</v>
       </c>
       <c r="D339" t="s">
-        <v>230</v>
+        <v>251</v>
       </c>
       <c r="E339" t="s">
         <v>4</v>
@@ -6921,7 +6923,7 @@
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="B341" s="1">
         <v>0.29166666666666669</v>
@@ -6955,16 +6957,16 @@
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B343" s="1">
-        <v>0.29166666666666669</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C343" s="1">
-        <v>0.99930555555555556</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="D343" t="s">
-        <v>251</v>
+        <v>230</v>
       </c>
       <c r="E343" t="s">
         <v>11</v>
@@ -6989,7 +6991,7 @@
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B345" s="1">
         <v>0.33333333333333331</v>
@@ -7023,7 +7025,7 @@
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B347" s="1">
         <v>0.33333333333333331</v>
@@ -7057,7 +7059,7 @@
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B349" s="1">
         <v>0.33333333333333331</v>
@@ -7091,7 +7093,7 @@
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B351" s="1">
         <v>0.33333333333333331</v>
@@ -7125,7 +7127,7 @@
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B353" s="1">
         <v>0.33333333333333331</v>
@@ -7159,7 +7161,7 @@
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B355" s="1">
         <v>0.33333333333333331</v>
@@ -7193,7 +7195,7 @@
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B357" s="1">
         <v>0.33333333333333331</v>
@@ -7227,7 +7229,7 @@
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B359" s="1">
         <v>0.33333333333333331</v>
@@ -7261,47 +7263,19 @@
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B361" s="1">
-        <v>0.33333333333333331</v>
+        <v>0.72916666666666663</v>
       </c>
       <c r="C361" s="1">
-        <v>0.66666666666666663</v>
+        <v>0.875</v>
       </c>
       <c r="D361" t="s">
-        <v>230</v>
+        <v>263</v>
       </c>
       <c r="E361" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A362" t="s">
-        <v>14</v>
-      </c>
-      <c r="B362" t="s">
-        <v>2</v>
-      </c>
-      <c r="C362" t="s">
-        <v>2</v>
-      </c>
-      <c r="D362" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A363" t="s">
-        <v>262</v>
-      </c>
-      <c r="B363" s="1">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="C363" s="1">
-        <v>0.875</v>
-      </c>
-      <c r="D363" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>